<commit_message>
create gender specific data sets
</commit_message>
<xml_diff>
--- a/Analyses/main study - LLM/output/G3/summaryGraphics_RR_adj.xlsx
+++ b/Analyses/main study - LLM/output/G3/summaryGraphics_RR_adj.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATEN\PHD\Article_SoftRobotIntervention\Analyses\main study - LLM\output\G3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATEN\PHD\Article_SoftRobotIntervention_2\Analyses\main study - LLM\output\G3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5D55F0-26F7-4EBB-B549-0AD4E63BF7B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B902FFF0-9E94-4478-B1E7-2D81EEB636FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,49 +37,49 @@
     <t>TP</t>
   </si>
   <si>
-    <t>Perceived technological possibilities for rescue robots encompass a range of benefits and risks, with participants differentiating between traditional rigid robots and flexible, electronic-free soft robots. Shared characteristics between rigid and soft robots include their potential to enhance search operations, provide essential supplies, and adapt to various situations. However, soft robots are distinguished by their unique attributes, such as their ability to provide food and water to victims immediately, care for victims during long rescue operations, and manage difficult conditions. In contrast, rigid robots are highlighted for their advanced technological features, including enhanced sensory capabilities, night vision, and air rescue, which enable them to perform specialized tasks, such as hacking doors and transmitting images. Rigid robots are also perceived as more effective in disaster response scenarios, with advantages in speed, efficiency, and continuous operation. Ultimately, the most significant arguments emphasize the potential of rescue robots to revolutionize disaster response by providing critical support in challenging environments, while also acknowledging the limitations and risks associated with their use.</t>
-  </si>
-  <si>
     <t>TL</t>
   </si>
   <si>
-    <t>Perceived technological limitations of rescue robots are a pressing concern, with participants differentiating between traditional rigid robots and flexible, electronic-free soft robots. While both types of robots share concerns related to potential errors in algorithms, operational duration, and energy sources, soft robots are uniquely characterized by their vulnerability to damage, limited robustness, and potential to get stuck. In contrast, rigid robots are perceived to have limited autonomy, restricted mobility, and a higher risk of faulty analyses. Notably, soft robots are seen as more prone to damage and less robust, whereas rigid robots are viewed as more specialized and limited in their adaptability to diverse rescue scenarios. Overall, the most significant arguments emphasize the need for improved robustness, adaptability, and human oversight in rescue robot technology to ensure effective and reliable performance in emergency situations.</t>
-  </si>
-  <si>
     <t>SA</t>
   </si>
   <si>
-    <t>Perceived safety is a critical aspect of rescue robots, with participants differentiating between traditional rigid robots and flexible, electronic-free soft robots. While both types of robots share characteristics such as enhanced operational efficiency, improved access to remote or hard-to-reach locations, and the ability to perform physical tasks beyond human capabilities, soft robots are distinguished by their unique attributes. Specifically, soft robots are designed to reduce the risk of injury to victims and rescuers, with their flexibility allowing them to access tight or narrow spaces and navigate challenging environments with lower risk. Furthermore, soft robots are perceived as more adaptable and reliable in hazardous conditions, with their organic construction method reducing the risk of injury and promoting a safer rescue operation. Overall, the perceived safety of rescue robots is significantly influenced by their design and capabilities, with rigid robots emphasizing strength, reliability, and operational efficiency, while soft robots prioritize adaptability, accessibility, and reduced risk of injury.</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
-    <t>Perceived risks associated with rescue robots are a crucial consideration in their development and deployment. Notably, both traditional rigid robots and flexible, electronic-free soft robots share concerns related to technical issues, accuracy, and safety. However, distinct differences emerge in the perceived risks between these two types of robots. Soft robots are particularly susceptible to durability concerns, with participants expressing worries about their fragility and potential for damage. In contrast, rigid robots are more likely to be associated with technical issues, potential misuse, and objective concerns, such as developmental errors and moral considerations. Furthermore, rigid robots are perceived to pose a greater risk of physical harm and misidentification of survivors. Soft robots, on the other hand, are distinguished by their unique attributes, including their potential for adaptability and flexibility in unpredictable rescue scenarios. Ultimately, understanding these perceived risks is essential for the development of effective and reliable rescue robots that can operate safely and efficiently in complex emergency situations.</t>
-  </si>
-  <si>
     <t>HRIP</t>
   </si>
   <si>
-    <t>Perceived positive Human-Robot-Interaction in rescue robots is characterized by sustained performance, collaborative support, and emotional resilience. Both traditional rigid robots and flexible, electronic-free soft robots share these essential attributes, ensuring reliable functionality and effective collaboration during rescue operations. However, soft robots distinguish themselves through their unique ability to provide emotional reassurance, leveraging their adaptable forms and non-mechanical appearance to offer comfort and calm to victims in distress. This distinctive feature, combined with their capacity to access and support individuals in hard-to-reach areas, underscores the significance of soft robots in rescue scenarios, ultimately highlighting the importance of considering the benefits of soft robot design in Human-Robot-Interaction for rescue applications.</t>
-  </si>
-  <si>
     <t>HRIN</t>
   </si>
   <si>
-    <t>Perceived negative Human-Robot-Interaction in rescue scenarios is a pressing concern, with participants expressing apprehensions regarding the emotional detachment of robots. Despite these concerns, both traditional rigid robots and flexible, electronic-free soft robots share common characteristics, such as the potential to evoke fear, mistrust, and emotional discomfort in victims. However, soft robots are distinguished by their unique attributes, which mitigate these negative perceptions. Notably, soft robots are perceived as less intimidating and more approachable, with participants expressing fewer concerns about emotional coldness, lack of emotional understanding, and reliance and trust. This is likely due to their non-threatening appearance and gentle, organic design. In contrast, rigid robots are viewed as more emotionally detached, lacking humanity, and incapable of providing the emotional support and closeness that victims may need. Overall, the most significant arguments suggest that the design of rescue robots should prioritize emotional understanding, empathy, and human-like interaction to alleviate perceived negative Human-Robot-Interaction and ensure effective rescue operations.</t>
-  </si>
-  <si>
     <t>AP</t>
   </si>
   <si>
-    <t>Perceived positive anthropomorphism in rescue robots is characterized by attributes that facilitate effective and efficient rescue operations. Both traditional rigid robots and flexible, electronic-free soft robots share characteristics that enable them to handle emotionally charged situations with logic and consistency, operate autonomously, and make decisions without human emotions and biases. However, soft robots are distinguished by their unique human-like design, which promotes emotional engagement, familiarity, and trust in their interactions. This natural, animal-like appearance fosters a sense of closeness, making them appear less artificial. In contrast, rigid robots are valued for their lack of emotionality, efficiency, and ability to make autonomous decisions, allowing them to perform tasks quickly and without fatigue. Overall, the most significant arguments suggest that while both types of robots have their advantages, rigid robots are perceived as more effective in high-stress rescue scenarios due to their operational efficiency and autonomy, whereas soft robots are seen as more relatable and trustworthy due to their human-like design.</t>
-  </si>
-  <si>
     <t>AN</t>
   </si>
   <si>
-    <t>Perceived negative anthropomorphism in rescue robots is a pressing concern, as it can significantly impact human-robot relationships and the effectiveness of rescue operations. Despite their differences, both traditional rigid robots and flexible, electronic-free soft robots share common characteristics, such as the potential to evoke feelings of unease due to their human-like features. However, soft robots are distinguished by their unique attributes, including their non-intimidating appearance and ability to provide a sense of comfort, which may alleviate concerns related to perceived negative anthropomorphism. In contrast, rigid robots are often viewed as inhuman, lacking empathy and human judgment, and prone to errors in autonomy, which can hinder their ability to provide effective emotional support and make optimal decisions in complex rescue scenarios. Overall, the most significant arguments suggest that the perceived negative anthropomorphism of rescue robots, particularly rigid ones, can have far-reaching consequences for human-robot relationships and the success of rescue missions, emphasizing the need for careful consideration of these factors in robot design and development.</t>
+    <t>The perceived technological possibilities of rescue robots are multifaceted, with participants highlighting various benefits and risks associated with their use in emergency response scenarios. Notably, the ability of robots to access and navigate locations that are challenging for humans to reach, such as unstable areas or rubble-filled buildings, is seen as a significant advantage. This is particularly true for soft robots, which are envisioned to provide essential supplies like food, water, and medicine to victims, thereby increasing their chances of survival. Additionally, the speed and effectiveness of task completion facilitated by rescue robots, including energy throughput and uninterrupted operations, are emphasized as key benefits. The potential for robots to perform specialized tasks beyond human capacity, such as flying, shrinking, and hacking doors, is also highlighted. Furthermore, the adaptability of rescue robots to various dangerous situations, such as extreme temperatures and physical conditions, is seen as crucial in disaster response scenarios. While concerns are raised about the current limitations of rescue robots in handling complex or multiple tasks simultaneously, their readiness and adaptability are emphasized as key advantages. Overall, the perceived technological possibilities of rescue robots, particularly soft robots, are centered around their ability to enhance information gathering, provide essential supplies, and perform tasks that exceed human capabilities in emergency situations.</t>
+  </si>
+  <si>
+    <t>The perceived technological limitations of rescue robots pose significant risks and benefits, with participants differentiating between traditional rigid robots and flexible, electronic-free soft robots. A primary concern revolves around the perceived risk of AI, with participants expressing skepticism about the ability of rescue robots to accurately assess complex situations compared to human judgment. This concern is closely tied to the risk of faulty analyses, where errors or inaccuracies in the analysis performed by rescue robots may occur due to reliance on recognition software. Furthermore, participants highlighted the limited autonomy of rescue robots, which may struggle to navigate unpredictable environments or adapt to dynamic circumstances due to their restricted decision-making abilities. In terms of shared perceptions, both rigid and soft robots are seen as having operational limitations, including concerns related to robot runtime, energy sources, and potential delays in rescue operations. However, soft robots are uniquely characterized by their vulnerability to damage, with participants expressing concerns about the durability, repairability, and longevity of these robots in critical situations. Notably, the soft material can damage quickly, raising questions about the robustness of soft robots. Despite these limitations, soft robots offer distinct advantages, including their potential for increased flexibility and adaptability in complex rescue scenarios. Ultimately, understanding the risks and benefits of perceived technological limitations is crucial for the development of effective rescue robots that can operate efficiently and safely in emergency situations.</t>
+  </si>
+  <si>
+    <t>The perceived safety of rescue robots is a critical aspect of their deployment, with participants differentiating between traditional rigid robots and flexible, electronic-free soft robots. The most significant benefit of rescue robots lies in their operational efficiency, with the ability to improve overall performance, reduce response times, and minimize risks to victims and rescuers through quicker and safer interventions. This is closely followed by their reliability, emphasizing consistent performance, precise control, and the role of rescue robots in reducing risks by ensuring dependable operation in hazardous conditions. Additionally, participants highlighted the physical capabilities of rescue robots, including their ability to perform tasks beyond human capabilities, such as lifting heavy objects and navigating difficult terrains. The accessibility of rescue robots, particularly in tight or narrow spaces, was also seen as a significant advantage, enhancing their utility and safety in rescue operations. While rigid robots were perceived as stronger and more reliable, soft robots were seen as more adaptable and flexible, with a lower risk of injury to victims and rescuers. The delivery of goods in hazardous environments and the ability to access remote or hard-to-reach locations were also identified as key benefits of rescue robots. Overall, the perceived safety of rescue robots is closely tied to their ability to operate effectively in hazardous environments, reduce risks to victims and rescuers, and provide a reliable and efficient means of conducting rescue operations.</t>
+  </si>
+  <si>
+    <t>The perceived risks associated with rescue robots vary significantly between traditional rigid robots and flexible, electronic-free soft robots. Notably, concerns about durability and material defects are significantly more pronounced for soft robots, with participants frequently expressing worries about their fragility and susceptibility to damage. In contrast, rigid robots are more likely to be associated with technical issues, potential misuse, and objective concerns, such as developmental errors and moral considerations. Both types of robots raise concerns about accuracy, with participants highlighting the potential for imprecision and limitations in performance under exceptional circumstances. However, soft robots are perceived as having unique attributes, including a higher risk of damage and material defects, which may impact their overall performance and effectiveness in rescue operations. Despite these differences, both rigid and soft robots share common concerns related to safety, potential physical harm, and misidentification, emphasizing the need for careful consideration and mitigation strategies to ensure their safe and effective deployment in emergency situations. Ultimately, the distinct characteristics of soft robots, including their flexibility and electronic-free design, introduce new challenges and opportunities that must be carefully weighed against their potential benefits in rescue operations.</t>
+  </si>
+  <si>
+    <t>In the context of Human-Robot-Interaction for rescue robots, participants emphasized the significance of collaborative support, where robots provide tangible assistance in rescue scenarios, enhancing human capabilities through collaboration and support rather than replacement. This aspect was deemed crucial for both traditional rigid robots and flexible, electronic-free soft robots, as they can work complementary to human activities and take care of people who are initially unreachable. Additionally, the importance of sustained performance was highlighted, focusing on the robots' physical and mental stamina during prolonged rescue operations. Notably, soft robots were perceived to offer emotional resilience through their design, adaptable forms, or demeanor, providing calm and optimism to victims in distress, which was not explicitly mentioned for rigid robots. Overall, the findings suggest that soft robots, with their unique attributes, may offer a more comprehensive support system in rescue operations, combining collaborative support, sustained performance, and emotional reassurance, which could have significant benefits for victims and rescue teams alike.</t>
+  </si>
+  <si>
+    <t>In the context of Human-Robot-Interaction for rescue robots, participants' perceptions of perceived negative interactions were largely driven by concerns about emotional detachment and lack of empathy. The most significant concerns revolved around the fear and discomfort caused by emotionally detached robots, with participants emphasizing the importance of human-like emotional understanding and empathy in rescue scenarios. This was particularly pronounced for traditional rigid robots, where participants expressed fears about the robots' lack of humanity, emotional coldness, and inability to recognize and respond to distress or fear. The absence of human-like emotional depth and compassion in these robots was seen as a significant limitation, with participants highlighting the need for emotional support and closeness during emergency situations. In contrast, flexible, electronic-free soft robots were perceived as less intimidating, with participants expressing irritation primarily due to their appearance. Notably, soft robots were not associated with the same level of emotional detachment and lack of empathy as their rigid counterparts, suggesting that their unique attributes may offer a more acceptable alternative for rescue operations. Overall, the findings underscore the importance of considering the emotional and social aspects of Human-Robot-Interaction in rescue scenarios, with soft robots potentially offering a more promising approach to addressing these concerns.</t>
+  </si>
+  <si>
+    <t>In the context of rescue robots, participants perceived benefits in the autonomous functioning of traditional rigid robots, which were seen as advantageous in high-stress situations due to their lack of emotionality, enabling them to handle emotionally charged scenarios with logic and consistency. This trait, combined with their efficiency in performing tasks quickly and without fatigue, made them well-suited for critical situations. Furthermore, the ability of rigid robots to make autonomous decisions, uninfluenced by human emotions and biases, was viewed as a significant advantage. In contrast, flexible, electronic-free soft robots were perceived as having a unique attribute - their human-like design, which promoted emotional engagement, familiarity, and trust in interactions. This natural, animal-like quality made them appear less artificial and more relatable, potentially fostering a sense of comfort and cooperation in rescue scenarios. Overall, while rigid robots excelled in their logical and efficient operation, soft robots offered a distinct advantage in their ability to establish emotional connections with humans, highlighting the importance of considering the benefits and risks of perceived positive anthropomorphism in rescue robot design.</t>
+  </si>
+  <si>
+    <t>The perceived negative anthropomorphism of rescue robots raises significant concerns regarding their effectiveness in providing emotional support and care in rescue scenarios. The most pressing issue is the lack of empathy, which is particularly pronounced in traditional rigid robots, where participants expressed concerns about the absence of emotional understanding, human closeness, and compassion. This limitation could hinder the robots' ability to provide emotional support, ultimately impacting the quality of care and human-robot relationships. Furthermore, participants noted that rigid robots' autonomous functioning may lead to errors in decision-making, lack of human judgment, and a perceived contradiction to rescue goals, which could compromise the success of rescue missions. In contrast, soft robots, with their flexible and electronic-free design, evoke a sense of unease due to their intimidating appearance, but participants did not express concerns about their lack of empathy or human judgment. Notably, both types of robots are perceived as lacking human involvement in interactions, with participants emphasizing the need for human intervention in decision-making processes. Overall, the findings suggest that the benefits of soft robots, such as their unique design, may be overshadowed by the risks associated with their perceived negative anthropomorphism, highlighting the need for further research into the development of empathetic and human-centered rescue robots.</t>
   </si>
 </sst>
 </file>
@@ -135,16 +135,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -450,111 +456,112 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="144.140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="144.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C5" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C6" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C7" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C8" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="5" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>